<commit_message>
Modificacion a la base de datos
</commit_message>
<xml_diff>
--- a/doc/Copia de Recintos Electorales C-51.xlsx
+++ b/doc/Copia de Recintos Electorales C-51.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sivo\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F1410BA-72DC-4ABA-982D-EE0D15BCB433}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0532D9-E54D-4AB0-8FBC-27112BBCCFA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="563" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2686,7 +2686,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2694,13 +2693,12 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2715,13 +2713,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2822,16 +2814,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -3113,6 +3105,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A3:K689"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -27083,13 +27076,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Hoja2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27851,7 +27844,7 @@
         <v>5743</v>
       </c>
     </row>
-    <row r="28" spans="2:10" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="23" t="s">
         <v>768</v>
       </c>
@@ -27909,7 +27902,7 @@
         <v>3798</v>
       </c>
     </row>
-    <row r="30" spans="2:10" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="23" t="s">
         <v>764</v>
       </c>
@@ -27938,7 +27931,7 @@
         <v>3121</v>
       </c>
     </row>
-    <row r="31" spans="2:10" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="23" t="s">
         <v>764</v>
       </c>
@@ -27967,7 +27960,7 @@
         <v>2328</v>
       </c>
     </row>
-    <row r="32" spans="2:10" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="23" t="s">
         <v>768</v>
       </c>
@@ -27996,7 +27989,7 @@
         <v>7417</v>
       </c>
     </row>
-    <row r="33" spans="2:10" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="23" t="s">
         <v>768</v>
       </c>
@@ -28054,7 +28047,7 @@
         <v>5258</v>
       </c>
     </row>
-    <row r="35" spans="2:10" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="23" t="s">
         <v>768</v>
       </c>
@@ -28083,7 +28076,7 @@
         <v>3165</v>
       </c>
     </row>
-    <row r="36" spans="2:10" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="23" t="s">
         <v>768</v>
       </c>
@@ -28141,7 +28134,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="38" spans="2:10" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="23" t="s">
         <v>768</v>
       </c>
@@ -28199,7 +28192,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="40" spans="2:10" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="23" t="s">
         <v>768</v>
       </c>
@@ -28228,7 +28221,7 @@
         <v>3950</v>
       </c>
     </row>
-    <row r="41" spans="2:10" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="23" t="s">
         <v>768</v>
       </c>
@@ -28257,7 +28250,7 @@
         <v>4815</v>
       </c>
     </row>
-    <row r="42" spans="2:10" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="23" t="s">
         <v>768</v>
       </c>
@@ -28286,7 +28279,7 @@
         <v>3089</v>
       </c>
     </row>
-    <row r="43" spans="2:10" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="23" t="s">
         <v>763</v>
       </c>
@@ -28315,7 +28308,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="44" spans="2:10" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="23" t="s">
         <v>763</v>
       </c>

</xml_diff>